<commit_message>
a few test scenario/test cases added
</commit_message>
<xml_diff>
--- a/Test documentation/03-TestSceanrio.xlsx
+++ b/Test documentation/03-TestSceanrio.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arthurbabenko/Documents/Testing/Java/Bestseller/Test documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F3B2824-23BC-9B46-8EB7-087D0E09D98B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F289D8A-41D0-814B-BBA2-564A799349F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" xr2:uid="{FDE17A92-904B-42F4-9FAD-C9666220B1F7}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" xr2:uid="{FDE17A92-904B-42F4-9FAD-C9666220B1F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Bestseller" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Test Scenario Description</t>
   </si>
@@ -85,6 +85,24 @@
   </si>
   <si>
     <t>Popup menu</t>
+  </si>
+  <si>
+    <t>Discount feature</t>
+  </si>
+  <si>
+    <t>Check order realise.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check whishlist Functionallity. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check sorting Functionallity. </t>
+  </si>
+  <si>
+    <t>BS2.1</t>
+  </si>
+  <si>
+    <t>Check filtrs Functionallity.</t>
   </si>
   <si>
     <r>
@@ -93,7 +111,7 @@
         <color rgb="FF00B050"/>
         <rFont val="Calibri (Body)"/>
       </rPr>
-      <t>1.	Check system behavior when valid email id and password is entered.  DONE</t>
+      <t>1.	Check system behavior when valid email id and password is entered.  AUTOMATIZATION DONE</t>
     </r>
     <r>
       <rPr>
@@ -113,7 +131,7 @@
         <color rgb="FF00B050"/>
         <rFont val="Calibri (Body)"/>
       </rPr>
-      <t>3.	Check system behavior when valid email id and invalid password is entered. DONE</t>
+      <t>3.	Check system behavior when valid email id and invalid password is entered. AUTOMATIZATION DONE</t>
     </r>
     <r>
       <rPr>
@@ -130,47 +148,38 @@
     </r>
   </si>
   <si>
-    <t>Discount feature</t>
-  </si>
-  <si>
-    <t>Check order realise.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Check system behavior when wrong card number is entered. DONE </t>
-  </si>
-  <si>
-    <t>1. Check if works discount "Two T-shirt for 90 zl" in Men section. DONE</t>
-  </si>
-  <si>
-    <t>1. Check if sorting are correct when choosing sort method from Highest to Low. DONE</t>
-  </si>
-  <si>
-    <t>1. Check if all elements displayed in popup menu in Kids section. DONE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check whishlist Functionallity. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check sorting Functionallity. </t>
-  </si>
-  <si>
-    <t>1. Check if all elements sucessfully added to whishlist. DONE</t>
-  </si>
-  <si>
-    <t>BS2.1</t>
-  </si>
-  <si>
-    <t>Check filtrs Functionallity.</t>
-  </si>
-  <si>
-    <t>1. Check if title from URL equals titles for Web API. DONE</t>
-  </si>
-  <si>
-    <t>1. Check if choosen filtrs are applyed and visible. DONE</t>
-  </si>
-  <si>
-    <t>1. After adding item to cart check if item still in cart after page refresh. DONE
-2. Check if items adding in cart after loggin. DONE</t>
+    <t>1. Check if title from URL equals titles for Web API. AUTOMATIZATION DONE</t>
+  </si>
+  <si>
+    <t>1. After adding item to cart check if item still in cart after page refresh. AUTOMATIZATION DONE
+2. Check if items adding in cart after loggin. AUTOMATIZATION DONE</t>
+  </si>
+  <si>
+    <t>1. Check if all elements displayed in popup menu in Kids section. AUTOMATIZATION DONE</t>
+  </si>
+  <si>
+    <t>1. Check if works discount "Two T-shirt for 90 zl" in Men section. AUTOMATIZATION DONE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Check system behavior when wrong card number is entered. AUTOMATIZATION DONE </t>
+  </si>
+  <si>
+    <t>1. Check if sorting are correct when choosing sort method from Highest to Low. AUTOMATIZATION DONE</t>
+  </si>
+  <si>
+    <t>1. Check if all elements sucessfully added to whishlist. AUTOMATIZATION DONE</t>
+  </si>
+  <si>
+    <t>1. Check if choosen filtrs are applyed and visible. AUTOMATIZATION DONE</t>
+  </si>
+  <si>
+    <t>1. Check search results for empty field.
+2. Check search with 5 spaces.
+3. Check search fields length max.
+4. Check search with word "marynarka"
+5. Check search by entering exist item number.
+6. Check search by entering non exist item number.
+7. Check search with special charackter.</t>
   </si>
 </sst>
 </file>
@@ -298,13 +307,13 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -626,7 +635,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -634,18 +643,18 @@
     <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="69.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="81.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="D1" s="4"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
     </row>
     <row r="3" spans="1:4" ht="16">
       <c r="A3" s="5" t="s">
@@ -672,10 +681,10 @@
         <v>2</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="112">
       <c r="A5" s="3">
         <v>2</v>
       </c>
@@ -685,7 +694,9 @@
       <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="1"/>
+      <c r="D5" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="3">
@@ -697,8 +708,8 @@
       <c r="C6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>31</v>
+      <c r="D6" s="7" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="32">
@@ -711,8 +722,8 @@
       <c r="C7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="9" t="s">
-        <v>33</v>
+      <c r="D7" s="8" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -725,8 +736,8 @@
       <c r="C8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>25</v>
+      <c r="D8" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -737,10 +748,10 @@
         <v>10</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>23</v>
+        <v>19</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -751,10 +762,10 @@
         <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -765,10 +776,10 @@
         <v>12</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -779,10 +790,10 @@
         <v>13</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>28</v>
+        <v>21</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -790,13 +801,13 @@
         <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>32</v>
+        <v>24</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:4">

</xml_diff>

<commit_message>
Test scenario and PageObject edited due to new tests created
</commit_message>
<xml_diff>
--- a/Test documentation/03-TestSceanrio.xlsx
+++ b/Test documentation/03-TestSceanrio.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arthurbabenko/Documents/Testing/Java/Bestseller/Test documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F289D8A-41D0-814B-BBA2-564A799349F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B81F24D5-8573-3F49-B738-B729941B2372}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" xr2:uid="{FDE17A92-904B-42F4-9FAD-C9666220B1F7}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" xr2:uid="{FDE17A92-904B-42F4-9FAD-C9666220B1F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Bestseller" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Test Scenario Description</t>
   </si>
@@ -103,49 +103,6 @@
   </si>
   <si>
     <t>Check filtrs Functionallity.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>1.	Check system behavior when valid email id and password is entered.  AUTOMATIZATION DONE</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-2.	Check system behavior when invalid email id and valid password is entered. 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri (Body)"/>
-      </rPr>
-      <t>3.	Check system behavior when valid email id and invalid password is entered. AUTOMATIZATION DONE</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-4.	Check system behavior when invalid email id and invalid password is entered. 
-5.	Check system behavior when email id and password are left blank and Sign in entered. 
-6.	Check Forgot your password is working as expected</t>
-    </r>
   </si>
   <si>
     <t>1. Check if title from URL equals titles for Web API. AUTOMATIZATION DONE</t>
@@ -180,6 +137,168 @@
 5. Check search by entering exist item number.
 6. Check search by entering non exist item number.
 7. Check search with special charackter.</t>
+  </si>
+  <si>
+    <t>BS2.2</t>
+  </si>
+  <si>
+    <t>Check order functionallity</t>
+  </si>
+  <si>
+    <t>1. Check with empty fields</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>1. Check system behavior when valid email id and password is entered.  AUTOMATIZATION DONE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">2. Check system behavior when invalid email id and valid password is entered. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>AUTOMATIZATION DONE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>3. Check system behavior when valid email id and invalid password is entered. AUTOMATIZATION DONE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>4. Check system behavior when invalid email id and invalid password is entered. AUTOMATIZATION DONE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>5. Check system behavior when email id and password are left blank and Sign in entered. AUTOMATIZATION DONE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>6. Check Forgot your password wihout email AUTOMATIZATION DONE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>7. Check Forgot your password wrong email type AUTOMATIZATION DONE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>8. Check Forgot your password is working as expected AUTOMATIZATION DONE</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -635,7 +754,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -643,7 +762,7 @@
     <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="81.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="89" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -670,7 +789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="96">
+    <row r="4" spans="1:4" ht="128">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -681,7 +800,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="112">
@@ -695,7 +814,7 @@
         <v>3</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -709,7 +828,7 @@
         <v>16</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="32">
@@ -723,7 +842,7 @@
         <v>17</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -737,7 +856,7 @@
         <v>18</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -751,7 +870,7 @@
         <v>19</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -765,7 +884,7 @@
         <v>20</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -779,7 +898,7 @@
         <v>22</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -793,7 +912,7 @@
         <v>21</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -807,16 +926,22 @@
         <v>24</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="3">
         <v>11</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="3">

</xml_diff>